<commit_message>
video records uploaded for lesson01 and lesson02
</commit_message>
<xml_diff>
--- a/src/main/java/az/et/_syllabus/course_details.xlsx
+++ b/src/main/java/az/et/_syllabus/course_details.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -37,7 +37,13 @@
     <t xml:space="preserve">Lesson #1</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=VHVTDQKvbmY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lesson #2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=s0h7LEcAF6Q </t>
   </si>
   <si>
     <t xml:space="preserve">Lesson #3</t>
@@ -64,7 +70,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yy"/>
+    <numFmt numFmtId="165" formatCode="d&quot;. &quot;mmm&quot;. &quot;yyyy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -108,16 +114,16 @@
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Cambria"/>
+      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
-      <name val="Cambria"/>
-      <family val="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -175,7 +181,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -192,7 +198,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -208,6 +214,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -220,7 +230,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -242,10 +252,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -329,7 +335,7 @@
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,99 +354,111 @@
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="11" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="n">
+    <row r="2" s="12" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
-      <c r="AMI2" s="12"/>
+      <c r="C2" s="10" t="n">
+        <v>44863</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="AMI2" s="13"/>
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="13" t="n">
+      <c r="A3" s="14" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="10" t="n">
+        <v>44867</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="16"/>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="13" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="14" t="s">
+      <c r="B6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="16"/>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="15"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="14" t="s">
+      <c r="B7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="n">
         <v>7</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="15"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
+      <c r="B8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="n">
         <v>8</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="15"/>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="9"/>
-      <c r="D8" s="15"/>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="15"/>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="16"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://www.youtube.com/watch?v=VHVTDQKvbmY"/>
+    <hyperlink ref="D3" r:id="rId2" display="https://www.youtube.com/watch?v=s0h7LEcAF6Q"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
all info with lesson15 attached
</commit_message>
<xml_diff>
--- a/src/main/java/az/et/_syllabus/course_details.xlsx
+++ b/src/main/java/az/et/_syllabus/course_details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>№</t>
   </si>
@@ -93,16 +93,31 @@
     <t>Lesson #11</t>
   </si>
   <si>
+    <t>https://youtu.be/w680kxUzdJ4</t>
+  </si>
+  <si>
     <t>Lesson #12</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Ha0lxiWJs8s</t>
   </si>
   <si>
     <t>Lesson #13</t>
   </si>
   <si>
+    <t>https://youtu.be/gbQ5G1-sg9A</t>
+  </si>
+  <si>
     <t>Lesson #14</t>
   </si>
   <si>
+    <t>https://youtu.be/Tk-5v7ElMyM</t>
+  </si>
+  <si>
     <t>Lesson #15</t>
+  </si>
+  <si>
+    <t>https://youtu.be/q5vxDFYG1nQ</t>
   </si>
   <si>
     <t>Lesson #16</t>
@@ -186,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -252,9 +267,6 @@
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -913,8 +925,12 @@
       <c r="B13" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="13"/>
+      <c r="C13" s="16">
+        <v>44909.0</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>25</v>
+      </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -943,10 +959,14 @@
         <v>4.0</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="14"/>
+      <c r="C14" s="16">
+        <v>44911.0</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
@@ -975,10 +995,14 @@
         <v>5.0</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="16">
+        <v>44918.0</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1007,10 +1031,14 @@
         <v>6.0</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="22"/>
+      <c r="C16" s="16">
+        <v>44923.0</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>31</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
@@ -1039,10 +1067,14 @@
         <v>7.0</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="22"/>
+      <c r="C17" s="16">
+        <v>44928.0</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>33</v>
+      </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
@@ -1071,10 +1103,10 @@
         <v>8.0</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C18" s="16"/>
-      <c r="D18" s="23"/>
+      <c r="D18" s="22"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -28605,10 +28637,15 @@
     <hyperlink r:id="rId7" ref="D9"/>
     <hyperlink r:id="rId8" ref="D11"/>
     <hyperlink r:id="rId9" ref="D12"/>
+    <hyperlink r:id="rId10" ref="D13"/>
+    <hyperlink r:id="rId11" ref="D14"/>
+    <hyperlink r:id="rId12" ref="D15"/>
+    <hyperlink r:id="rId13" ref="D16"/>
+    <hyperlink r:id="rId14" ref="D17"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait"/>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>